<commit_message>
Added more input data
</commit_message>
<xml_diff>
--- a/For_Kasper__From_France.xlsx
+++ b/For_Kasper__From_France.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaspe\Documents\GitHub\PCA_Analysis_ACS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaspe\Documents\GitHub\ACS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCE4AA7-0E0D-4BED-A451-D2E0023AC839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC370A1-28C7-4888-95BB-16121338787C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -465,8 +465,8 @@
   <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3926,15 +3926,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010038D734F0F3A5BC4B93067F435B8A0367" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dc2a69a662d1e6afe884a6c3f7e677ba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a2c3285d-3169-4fd7-bb15-31b8821600b8" xmlns:ns3="d680cd0c-a5a7-487b-9fb0-cd842ef4bb7b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="73968b4a3c12ae32bc653d2cad1f82ad" ns2:_="" ns3:_="">
     <xsd:import namespace="a2c3285d-3169-4fd7-bb15-31b8821600b8"/>
@@ -4137,6 +4128,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4149,14 +4149,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{092C2FD1-D057-4EED-9766-40D7FA57F18F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11797CC0-2A8E-44EB-AB7F-2B032C1A5135}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4171,6 +4163,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{092C2FD1-D057-4EED-9766-40D7FA57F18F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>